<commit_message>
Atualização do exercicos aula 11
</commit_message>
<xml_diff>
--- a/Exercicios_1/Mapa_Habilidades_EBAC_[Eric Douglas F Faria].xlsx
+++ b/Exercicios_1/Mapa_Habilidades_EBAC_[Eric Douglas F Faria].xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MEUS DOCUMENTOS\DOCUMENTOS ERIC\CURSOS\EBAC\TESTE DE SOFTWARE\Exercicios 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MEUS DOCUMENTOS\DOCUMENTOS ERIC\CURSOS\EBAC\EXERCICIOS_EBAC_2023\Exercicios_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88BB39BF-CCCC-43A5-ACC7-E648F25EA2CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F3574CA-7255-4DB7-811C-8FDE7354504F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="109">
   <si>
     <t>Legenda</t>
   </si>
@@ -357,6 +357,12 @@
   <si>
     <t>Grande Objetivo:</t>
   </si>
+  <si>
+    <t>Concluido</t>
+  </si>
+  <si>
+    <t>Não Concluido</t>
+  </si>
 </sst>
 </file>
 
@@ -567,14 +573,13 @@
     </font>
     <font>
       <b/>
-      <u/>
       <sz val="26"/>
       <color theme="7"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -629,8 +634,20 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -773,6 +790,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -904,6 +941,62 @@
     <xf numFmtId="0" fontId="11" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="23" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="23" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="23" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="23" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="24" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -928,11 +1021,11 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -943,11 +1036,17 @@
     <xf numFmtId="0" fontId="17" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -982,82 +1081,8 @@
     <xf numFmtId="0" fontId="20" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="23" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="23" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="23" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="23" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="24" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1065,8 +1090,24 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2648,20 +2689,20 @@
       <c r="C1" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="D1" s="45">
+      <c r="D1" s="65">
         <v>45005</v>
       </c>
-      <c r="E1" s="46"/>
-      <c r="F1" s="47"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="67"/>
     </row>
     <row r="3" spans="1:12" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="70" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
       <c r="F3" s="18"/>
       <c r="G3" s="18"/>
     </row>
@@ -2688,7 +2729,7 @@
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="64" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="27" t="s">
@@ -2706,7 +2747,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="44"/>
+      <c r="A7" s="64"/>
       <c r="B7" s="27" t="s">
         <v>55</v>
       </c>
@@ -2722,7 +2763,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="44"/>
+      <c r="A8" s="64"/>
       <c r="B8" s="27" t="s">
         <v>24</v>
       </c>
@@ -2738,7 +2779,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="44"/>
+      <c r="A9" s="64"/>
       <c r="B9" s="27" t="s">
         <v>58</v>
       </c>
@@ -2754,7 +2795,7 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="44"/>
+      <c r="A10" s="64"/>
       <c r="B10" s="27" t="s">
         <v>52</v>
       </c>
@@ -2770,7 +2811,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="44"/>
+      <c r="A11" s="64"/>
       <c r="B11" s="27" t="s">
         <v>12</v>
       </c>
@@ -2786,7 +2827,7 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="44"/>
+      <c r="A12" s="64"/>
       <c r="B12" s="27" t="s">
         <v>13</v>
       </c>
@@ -2802,7 +2843,7 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="44"/>
+      <c r="A13" s="64"/>
       <c r="B13" s="27" t="s">
         <v>10</v>
       </c>
@@ -2818,7 +2859,7 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="44"/>
+      <c r="A14" s="64"/>
       <c r="B14" s="27" t="s">
         <v>28</v>
       </c>
@@ -2834,7 +2875,7 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="44"/>
+      <c r="A15" s="64"/>
       <c r="B15" s="27" t="s">
         <v>56</v>
       </c>
@@ -2850,7 +2891,7 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="44"/>
+      <c r="A16" s="64"/>
       <c r="B16" s="29" t="s">
         <v>8</v>
       </c>
@@ -2866,7 +2907,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="44"/>
+      <c r="A17" s="64"/>
       <c r="B17" s="30" t="s">
         <v>50</v>
       </c>
@@ -2882,7 +2923,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="44"/>
+      <c r="A18" s="64"/>
       <c r="B18" s="27" t="s">
         <v>51</v>
       </c>
@@ -2898,7 +2939,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="44"/>
+      <c r="A19" s="64"/>
       <c r="B19" s="27" t="s">
         <v>9</v>
       </c>
@@ -2914,7 +2955,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="44"/>
+      <c r="A20" s="64"/>
       <c r="B20" s="27" t="s">
         <v>57</v>
       </c>
@@ -2930,7 +2971,7 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="44"/>
+      <c r="A21" s="64"/>
       <c r="B21" s="27" t="s">
         <v>11</v>
       </c>
@@ -2946,7 +2987,7 @@
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="44"/>
+      <c r="A22" s="64"/>
       <c r="B22" s="27" t="s">
         <v>27</v>
       </c>
@@ -2962,7 +3003,7 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="44"/>
+      <c r="A23" s="64"/>
       <c r="B23" s="27" t="s">
         <v>60</v>
       </c>
@@ -2978,7 +3019,7 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="44"/>
+      <c r="A24" s="64"/>
       <c r="B24" s="27" t="s">
         <v>61</v>
       </c>
@@ -2994,7 +3035,7 @@
       </c>
     </row>
     <row r="25" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="48" t="s">
+      <c r="A25" s="68" t="s">
         <v>14</v>
       </c>
       <c r="B25" s="31" t="s">
@@ -3012,7 +3053,7 @@
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="48"/>
+      <c r="A26" s="68"/>
       <c r="B26" s="31" t="s">
         <v>54</v>
       </c>
@@ -3028,7 +3069,7 @@
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="48"/>
+      <c r="A27" s="68"/>
       <c r="B27" s="31" t="s">
         <v>62</v>
       </c>
@@ -3044,7 +3085,7 @@
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="48"/>
+      <c r="A28" s="68"/>
       <c r="B28" s="31" t="s">
         <v>16</v>
       </c>
@@ -3060,7 +3101,7 @@
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="48"/>
+      <c r="A29" s="68"/>
       <c r="B29" s="31" t="s">
         <v>63</v>
       </c>
@@ -3074,15 +3115,15 @@
       <c r="E29" s="7">
         <v>2.5</v>
       </c>
-      <c r="G29" s="49" t="s">
+      <c r="G29" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="H29" s="49"/>
-      <c r="I29" s="49"/>
-      <c r="J29" s="49"/>
+      <c r="H29" s="69"/>
+      <c r="I29" s="69"/>
+      <c r="J29" s="69"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="48"/>
+      <c r="A30" s="68"/>
       <c r="B30" s="31" t="s">
         <v>17</v>
       </c>
@@ -3110,7 +3151,7 @@
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="48"/>
+      <c r="A31" s="68"/>
       <c r="B31" s="31" t="s">
         <v>25</v>
       </c>
@@ -3126,7 +3167,7 @@
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="48"/>
+      <c r="A32" s="68"/>
       <c r="B32" s="31" t="s">
         <v>53</v>
       </c>
@@ -3142,7 +3183,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="48"/>
+      <c r="A33" s="68"/>
       <c r="B33" s="31" t="s">
         <v>18</v>
       </c>
@@ -3158,7 +3199,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="48"/>
+      <c r="A34" s="68"/>
       <c r="B34" s="31" t="s">
         <v>19</v>
       </c>
@@ -3174,7 +3215,7 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="48"/>
+      <c r="A35" s="68"/>
       <c r="B35" s="32" t="s">
         <v>20</v>
       </c>
@@ -3190,7 +3231,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="48"/>
+      <c r="A36" s="68"/>
       <c r="B36" s="32" t="s">
         <v>21</v>
       </c>
@@ -3206,7 +3247,7 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="48"/>
+      <c r="A37" s="68"/>
       <c r="B37" s="32" t="s">
         <v>22</v>
       </c>
@@ -3281,8 +3322,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF37A969-82CF-C144-AD1B-458A8A931276}">
   <dimension ref="A1:AA1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3295,23 +3336,23 @@
     <col min="7" max="7" width="15.85546875" style="17" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27.85546875" style="17" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="31.7109375" style="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" style="17"/>
+    <col min="10" max="10" width="15.42578125" style="17" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13" style="17" customWidth="1"/>
     <col min="12" max="16384" width="10.85546875" style="17"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="98" t="s">
+      <c r="A1" s="92" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="98"/>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
-      <c r="G1" s="98"/>
-      <c r="H1" s="98"/>
-      <c r="I1" s="99"/>
+      <c r="B1" s="92"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
+      <c r="G1" s="92"/>
+      <c r="H1" s="92"/>
+      <c r="I1" s="93"/>
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
       <c r="L1" s="16"/>
@@ -3332,16 +3373,16 @@
       <c r="AA1" s="16"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A2" s="53"/>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="16"/>
+      <c r="A2" s="94"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="95"/>
+      <c r="J2" s="95"/>
       <c r="M2" s="16"/>
       <c r="N2" s="16"/>
       <c r="O2" s="16"/>
@@ -3353,32 +3394,34 @@
       <c r="U2" s="16"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="79" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="79" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="79" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="51" t="s">
+      <c r="D3" s="79" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="51" t="s">
+      <c r="E3" s="79" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51" t="s">
+      <c r="F3" s="79"/>
+      <c r="G3" s="79" t="s">
         <v>67</v>
       </c>
-      <c r="H3" s="51" t="s">
+      <c r="H3" s="79" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="52" t="s">
+      <c r="I3" s="91" t="s">
         <v>48</v>
       </c>
-      <c r="J3" s="16"/>
+      <c r="J3" s="91" t="s">
+        <v>107</v>
+      </c>
       <c r="L3" s="16"/>
       <c r="M3" s="16"/>
       <c r="N3" s="16"/>
@@ -3397,20 +3440,20 @@
       <c r="AA3" s="16"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A4" s="56"/>
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
+      <c r="A4" s="79"/>
+      <c r="B4" s="79"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
       <c r="E4" s="22" t="s">
         <v>49</v>
       </c>
       <c r="F4" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="52"/>
-      <c r="J4" s="16"/>
+      <c r="G4" s="79"/>
+      <c r="H4" s="79"/>
+      <c r="I4" s="91"/>
+      <c r="J4" s="91"/>
       <c r="K4" s="36"/>
       <c r="M4" s="16"/>
       <c r="N4" s="16"/>
@@ -3428,750 +3471,755 @@
       <c r="Z4" s="16"/>
       <c r="AA4" s="16"/>
     </row>
-    <row r="5" spans="1:27" s="76" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="69">
+    <row r="5" spans="1:27" s="50" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="44">
         <v>1</v>
       </c>
-      <c r="B5" s="70" t="s">
+      <c r="B5" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="C5" s="71" t="s">
+      <c r="C5" s="46" t="s">
         <v>94</v>
       </c>
-      <c r="D5" s="86" t="s">
+      <c r="D5" s="57" t="s">
         <v>100</v>
       </c>
-      <c r="E5" s="87">
+      <c r="E5" s="58">
         <v>45017</v>
       </c>
-      <c r="F5" s="87">
+      <c r="F5" s="58">
         <v>46148</v>
       </c>
-      <c r="G5" s="71" t="s">
+      <c r="G5" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="H5" s="73" t="s">
+      <c r="H5" s="48" t="s">
         <v>102</v>
       </c>
-      <c r="I5" s="74">
+      <c r="I5" s="49">
         <v>10800</v>
       </c>
-      <c r="J5" s="75"/>
-      <c r="K5" s="89"/>
-      <c r="M5" s="77"/>
-      <c r="N5" s="77"/>
-      <c r="O5" s="77"/>
-      <c r="P5" s="77"/>
-      <c r="Q5" s="77"/>
-      <c r="R5" s="77"/>
-      <c r="S5" s="77"/>
-      <c r="T5" s="77"/>
-      <c r="U5" s="77"/>
-      <c r="V5" s="77"/>
-      <c r="W5" s="77"/>
-      <c r="X5" s="77"/>
-      <c r="Y5" s="77"/>
-      <c r="Z5" s="77"/>
-      <c r="AA5" s="77"/>
-    </row>
-    <row r="6" spans="1:27" s="76" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="69">
+      <c r="J5" s="44"/>
+      <c r="K5" s="60"/>
+      <c r="M5" s="51"/>
+      <c r="N5" s="51"/>
+      <c r="O5" s="51"/>
+      <c r="P5" s="51"/>
+      <c r="Q5" s="51"/>
+      <c r="R5" s="51"/>
+      <c r="S5" s="51"/>
+      <c r="T5" s="51"/>
+      <c r="U5" s="51"/>
+      <c r="V5" s="51"/>
+      <c r="W5" s="51"/>
+      <c r="X5" s="51"/>
+      <c r="Y5" s="51"/>
+      <c r="Z5" s="51"/>
+      <c r="AA5" s="51"/>
+    </row>
+    <row r="6" spans="1:27" s="50" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="44">
         <v>2</v>
       </c>
-      <c r="B6" s="70" t="s">
+      <c r="B6" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="C6" s="71" t="s">
+      <c r="C6" s="46" t="s">
         <v>94</v>
       </c>
-      <c r="D6" s="86" t="s">
+      <c r="D6" s="57" t="s">
         <v>100</v>
       </c>
-      <c r="E6" s="87">
+      <c r="E6" s="58">
         <v>45017</v>
       </c>
-      <c r="F6" s="87">
+      <c r="F6" s="58">
         <v>45290</v>
       </c>
-      <c r="G6" s="71" t="s">
+      <c r="G6" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="H6" s="73" t="s">
+      <c r="H6" s="48" t="s">
         <v>101</v>
       </c>
-      <c r="I6" s="74">
+      <c r="I6" s="49">
         <v>2550</v>
       </c>
-      <c r="J6" s="75"/>
-      <c r="M6" s="77"/>
-      <c r="N6" s="77"/>
-      <c r="O6" s="77"/>
-      <c r="P6" s="77"/>
-      <c r="Q6" s="77"/>
-      <c r="R6" s="77"/>
-      <c r="S6" s="77"/>
-      <c r="T6" s="77"/>
-      <c r="U6" s="77"/>
-      <c r="V6" s="77"/>
-      <c r="W6" s="77"/>
-      <c r="X6" s="77"/>
-      <c r="Y6" s="77"/>
-      <c r="Z6" s="77"/>
-      <c r="AA6" s="77"/>
-    </row>
-    <row r="7" spans="1:27" s="76" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="69">
+      <c r="J6" s="44"/>
+      <c r="M6" s="51"/>
+      <c r="N6" s="51"/>
+      <c r="O6" s="51"/>
+      <c r="P6" s="51"/>
+      <c r="Q6" s="51"/>
+      <c r="R6" s="51"/>
+      <c r="S6" s="51"/>
+      <c r="T6" s="51"/>
+      <c r="U6" s="51"/>
+      <c r="V6" s="51"/>
+      <c r="W6" s="51"/>
+      <c r="X6" s="51"/>
+      <c r="Y6" s="51"/>
+      <c r="Z6" s="51"/>
+      <c r="AA6" s="51"/>
+    </row>
+    <row r="7" spans="1:27" s="50" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A7" s="44">
         <v>3</v>
       </c>
-      <c r="B7" s="70" t="s">
+      <c r="B7" s="45" t="s">
         <v>96</v>
       </c>
-      <c r="C7" s="71" t="s">
+      <c r="C7" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="D7" s="86" t="s">
+      <c r="D7" s="57" t="s">
         <v>100</v>
       </c>
-      <c r="E7" s="87">
+      <c r="E7" s="58">
         <v>45017</v>
       </c>
-      <c r="F7" s="87">
+      <c r="F7" s="58">
         <v>45290</v>
       </c>
-      <c r="G7" s="71" t="s">
+      <c r="G7" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="H7" s="73" t="s">
+      <c r="H7" s="48" t="s">
         <v>103</v>
       </c>
-      <c r="I7" s="74">
+      <c r="I7" s="49">
         <v>79.900000000000006</v>
       </c>
-      <c r="J7" s="75"/>
-      <c r="M7" s="77"/>
-      <c r="N7" s="77"/>
-      <c r="O7" s="77"/>
-      <c r="P7" s="77"/>
-      <c r="Q7" s="77"/>
-      <c r="R7" s="77"/>
-      <c r="S7" s="77"/>
-      <c r="T7" s="77"/>
-      <c r="U7" s="77"/>
-      <c r="V7" s="77"/>
-      <c r="W7" s="77"/>
-      <c r="X7" s="77"/>
-      <c r="Y7" s="77"/>
-      <c r="Z7" s="77"/>
-      <c r="AA7" s="77"/>
-    </row>
-    <row r="8" spans="1:27" s="76" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="69">
+      <c r="J7" s="44"/>
+      <c r="M7" s="51"/>
+      <c r="N7" s="51"/>
+      <c r="O7" s="51"/>
+      <c r="P7" s="51"/>
+      <c r="Q7" s="51"/>
+      <c r="R7" s="51"/>
+      <c r="S7" s="51"/>
+      <c r="T7" s="51"/>
+      <c r="U7" s="51"/>
+      <c r="V7" s="51"/>
+      <c r="W7" s="51"/>
+      <c r="X7" s="51"/>
+      <c r="Y7" s="51"/>
+      <c r="Z7" s="51"/>
+      <c r="AA7" s="51"/>
+    </row>
+    <row r="8" spans="1:27" s="50" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A8" s="44">
         <v>4</v>
       </c>
-      <c r="B8" s="70" t="s">
+      <c r="B8" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="C8" s="71" t="s">
+      <c r="C8" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="D8" s="86" t="s">
+      <c r="D8" s="57" t="s">
         <v>100</v>
       </c>
-      <c r="E8" s="87">
+      <c r="E8" s="58">
         <v>45017</v>
       </c>
-      <c r="F8" s="87">
+      <c r="F8" s="58">
         <v>45290</v>
       </c>
-      <c r="G8" s="71" t="s">
+      <c r="G8" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="H8" s="73" t="s">
+      <c r="H8" s="48" t="s">
         <v>103</v>
       </c>
-      <c r="I8" s="74">
+      <c r="I8" s="49">
         <v>79.900000000000006</v>
       </c>
-      <c r="J8" s="75"/>
-      <c r="M8" s="77"/>
-      <c r="N8" s="77"/>
-      <c r="O8" s="77"/>
-      <c r="P8" s="77"/>
-      <c r="Q8" s="77"/>
-      <c r="R8" s="77"/>
-      <c r="S8" s="77"/>
-      <c r="T8" s="77"/>
-      <c r="U8" s="77"/>
-      <c r="V8" s="77"/>
-      <c r="W8" s="77"/>
-      <c r="X8" s="77"/>
-      <c r="Y8" s="77"/>
-      <c r="Z8" s="77"/>
-      <c r="AA8" s="77"/>
-    </row>
-    <row r="9" spans="1:27" s="76" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="69">
+      <c r="J8" s="44"/>
+      <c r="M8" s="51"/>
+      <c r="N8" s="51"/>
+      <c r="O8" s="51"/>
+      <c r="P8" s="51"/>
+      <c r="Q8" s="51"/>
+      <c r="R8" s="51"/>
+      <c r="S8" s="51"/>
+      <c r="T8" s="51"/>
+      <c r="U8" s="51"/>
+      <c r="V8" s="51"/>
+      <c r="W8" s="51"/>
+      <c r="X8" s="51"/>
+      <c r="Y8" s="51"/>
+      <c r="Z8" s="51"/>
+      <c r="AA8" s="51"/>
+    </row>
+    <row r="9" spans="1:27" s="50" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A9" s="44">
         <v>5</v>
       </c>
-      <c r="B9" s="70" t="s">
+      <c r="B9" s="45" t="s">
         <v>98</v>
       </c>
-      <c r="C9" s="71" t="s">
+      <c r="C9" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="D9" s="86" t="s">
+      <c r="D9" s="57" t="s">
         <v>100</v>
       </c>
-      <c r="E9" s="87">
+      <c r="E9" s="58">
         <v>45017</v>
       </c>
-      <c r="F9" s="87">
+      <c r="F9" s="58">
         <v>45290</v>
       </c>
-      <c r="G9" s="71" t="s">
+      <c r="G9" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="H9" s="73" t="s">
+      <c r="H9" s="48" t="s">
         <v>103</v>
       </c>
-      <c r="I9" s="74">
+      <c r="I9" s="49">
         <v>79.900000000000006</v>
       </c>
-      <c r="J9" s="75"/>
-      <c r="M9" s="77"/>
-      <c r="N9" s="77"/>
-      <c r="O9" s="77"/>
-      <c r="P9" s="77"/>
-      <c r="Q9" s="77"/>
-      <c r="R9" s="77"/>
-      <c r="S9" s="77"/>
-      <c r="T9" s="77"/>
-      <c r="U9" s="77"/>
-      <c r="V9" s="77"/>
-      <c r="W9" s="77"/>
-      <c r="X9" s="77"/>
-      <c r="Y9" s="77"/>
-      <c r="Z9" s="77"/>
-      <c r="AA9" s="77"/>
-    </row>
-    <row r="10" spans="1:27" s="76" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="69">
+      <c r="J9" s="44"/>
+      <c r="M9" s="51"/>
+      <c r="N9" s="51"/>
+      <c r="O9" s="51"/>
+      <c r="P9" s="51"/>
+      <c r="Q9" s="51"/>
+      <c r="R9" s="51"/>
+      <c r="S9" s="51"/>
+      <c r="T9" s="51"/>
+      <c r="U9" s="51"/>
+      <c r="V9" s="51"/>
+      <c r="W9" s="51"/>
+      <c r="X9" s="51"/>
+      <c r="Y9" s="51"/>
+      <c r="Z9" s="51"/>
+      <c r="AA9" s="51"/>
+    </row>
+    <row r="10" spans="1:27" s="50" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A10" s="44">
         <v>6</v>
       </c>
-      <c r="B10" s="70" t="s">
+      <c r="B10" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="C10" s="71" t="s">
+      <c r="C10" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="D10" s="86" t="s">
+      <c r="D10" s="57" t="s">
         <v>100</v>
       </c>
-      <c r="E10" s="87">
+      <c r="E10" s="58">
         <v>45017</v>
       </c>
-      <c r="F10" s="87">
+      <c r="F10" s="58">
         <v>45290</v>
       </c>
-      <c r="G10" s="71" t="s">
+      <c r="G10" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="H10" s="73" t="s">
+      <c r="H10" s="48" t="s">
         <v>103</v>
       </c>
-      <c r="I10" s="74">
+      <c r="I10" s="49">
         <v>79.900000000000006</v>
       </c>
-      <c r="J10" s="75"/>
-      <c r="M10" s="77"/>
-      <c r="N10" s="77"/>
-      <c r="O10" s="77"/>
-      <c r="P10" s="77"/>
-      <c r="Q10" s="77"/>
-      <c r="R10" s="77"/>
-      <c r="S10" s="77"/>
-      <c r="T10" s="77"/>
-      <c r="U10" s="77"/>
-      <c r="V10" s="77"/>
-      <c r="W10" s="77"/>
-      <c r="X10" s="77"/>
-      <c r="Y10" s="77"/>
-      <c r="Z10" s="77"/>
-      <c r="AA10" s="77"/>
-    </row>
-    <row r="11" spans="1:27" s="76" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="69">
+      <c r="J10" s="44"/>
+      <c r="M10" s="51"/>
+      <c r="N10" s="51"/>
+      <c r="O10" s="51"/>
+      <c r="P10" s="51"/>
+      <c r="Q10" s="51"/>
+      <c r="R10" s="51"/>
+      <c r="S10" s="51"/>
+      <c r="T10" s="51"/>
+      <c r="U10" s="51"/>
+      <c r="V10" s="51"/>
+      <c r="W10" s="51"/>
+      <c r="X10" s="51"/>
+      <c r="Y10" s="51"/>
+      <c r="Z10" s="51"/>
+      <c r="AA10" s="51"/>
+    </row>
+    <row r="11" spans="1:27" s="50" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A11" s="44">
         <v>7</v>
       </c>
-      <c r="B11" s="70" t="s">
+      <c r="B11" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="C11" s="71" t="s">
+      <c r="C11" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="D11" s="100" t="s">
+      <c r="D11" s="63" t="s">
         <v>100</v>
       </c>
-      <c r="E11" s="87">
+      <c r="E11" s="58">
         <v>45017</v>
       </c>
-      <c r="F11" s="87">
+      <c r="F11" s="58">
         <v>45290</v>
       </c>
-      <c r="G11" s="71" t="s">
+      <c r="G11" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="H11" s="73" t="s">
+      <c r="H11" s="48" t="s">
         <v>103</v>
       </c>
-      <c r="I11" s="74">
+      <c r="I11" s="49">
         <v>79.900000000000006</v>
       </c>
-      <c r="J11" s="75"/>
-      <c r="M11" s="77"/>
-      <c r="N11" s="77"/>
-      <c r="O11" s="77"/>
-      <c r="P11" s="77"/>
-      <c r="Q11" s="77"/>
-      <c r="R11" s="77"/>
-      <c r="S11" s="77"/>
-      <c r="T11" s="77"/>
-      <c r="U11" s="77"/>
-      <c r="V11" s="77"/>
-      <c r="W11" s="77"/>
-      <c r="X11" s="77"/>
-      <c r="Y11" s="77"/>
-      <c r="Z11" s="77"/>
-      <c r="AA11" s="77"/>
-    </row>
-    <row r="12" spans="1:27" s="76" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="69">
+      <c r="J11" s="44"/>
+      <c r="M11" s="51"/>
+      <c r="N11" s="51"/>
+      <c r="O11" s="51"/>
+      <c r="P11" s="51"/>
+      <c r="Q11" s="51"/>
+      <c r="R11" s="51"/>
+      <c r="S11" s="51"/>
+      <c r="T11" s="51"/>
+      <c r="U11" s="51"/>
+      <c r="V11" s="51"/>
+      <c r="W11" s="51"/>
+      <c r="X11" s="51"/>
+      <c r="Y11" s="51"/>
+      <c r="Z11" s="51"/>
+      <c r="AA11" s="51"/>
+    </row>
+    <row r="12" spans="1:27" s="50" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="44">
         <v>8</v>
       </c>
-      <c r="B12" s="70" t="s">
+      <c r="B12" s="45" t="s">
         <v>91</v>
       </c>
-      <c r="C12" s="71" t="s">
+      <c r="C12" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="D12" s="86" t="s">
+      <c r="D12" s="57" t="s">
         <v>100</v>
       </c>
-      <c r="E12" s="87">
+      <c r="E12" s="58">
         <v>45017</v>
       </c>
-      <c r="F12" s="87">
+      <c r="F12" s="58">
         <v>45290</v>
       </c>
-      <c r="G12" s="71" t="s">
+      <c r="G12" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="H12" s="73" t="s">
+      <c r="H12" s="48" t="s">
         <v>103</v>
       </c>
-      <c r="I12" s="74">
+      <c r="I12" s="49">
         <v>79.900000000000006</v>
       </c>
-      <c r="J12" s="75"/>
-      <c r="M12" s="77"/>
-      <c r="N12" s="77"/>
-      <c r="O12" s="77"/>
-      <c r="P12" s="77"/>
-      <c r="Q12" s="77"/>
-      <c r="R12" s="77"/>
-      <c r="S12" s="77"/>
-      <c r="T12" s="77"/>
-      <c r="U12" s="77"/>
-      <c r="V12" s="77"/>
-      <c r="W12" s="77"/>
-      <c r="X12" s="77"/>
-      <c r="Y12" s="77"/>
-      <c r="Z12" s="77"/>
-      <c r="AA12" s="77"/>
-    </row>
-    <row r="13" spans="1:27" s="76" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="69">
+      <c r="J12" s="44"/>
+      <c r="M12" s="51"/>
+      <c r="N12" s="51"/>
+      <c r="O12" s="51"/>
+      <c r="P12" s="51"/>
+      <c r="Q12" s="51"/>
+      <c r="R12" s="51"/>
+      <c r="S12" s="51"/>
+      <c r="T12" s="51"/>
+      <c r="U12" s="51"/>
+      <c r="V12" s="51"/>
+      <c r="W12" s="51"/>
+      <c r="X12" s="51"/>
+      <c r="Y12" s="51"/>
+      <c r="Z12" s="51"/>
+      <c r="AA12" s="51"/>
+    </row>
+    <row r="13" spans="1:27" s="50" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="44">
         <v>9</v>
       </c>
-      <c r="B13" s="70" t="s">
+      <c r="B13" s="45" t="s">
         <v>92</v>
       </c>
-      <c r="C13" s="71" t="s">
+      <c r="C13" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="D13" s="86" t="s">
+      <c r="D13" s="57" t="s">
         <v>100</v>
       </c>
-      <c r="E13" s="87">
+      <c r="E13" s="58">
         <v>45017</v>
       </c>
-      <c r="F13" s="87">
+      <c r="F13" s="58">
         <v>45290</v>
       </c>
-      <c r="G13" s="71" t="s">
+      <c r="G13" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="H13" s="73" t="s">
+      <c r="H13" s="48" t="s">
         <v>103</v>
       </c>
-      <c r="I13" s="74">
+      <c r="I13" s="49">
         <v>79.900000000000006</v>
       </c>
-      <c r="J13" s="75"/>
-      <c r="M13" s="77"/>
-      <c r="N13" s="77"/>
-      <c r="O13" s="77"/>
-      <c r="P13" s="77"/>
-      <c r="Q13" s="77"/>
-      <c r="R13" s="77"/>
-      <c r="S13" s="77"/>
-      <c r="T13" s="77"/>
-      <c r="U13" s="77"/>
-      <c r="V13" s="77"/>
-      <c r="W13" s="77"/>
-      <c r="X13" s="77"/>
-      <c r="Y13" s="77"/>
-      <c r="Z13" s="77"/>
-      <c r="AA13" s="77"/>
-    </row>
-    <row r="14" spans="1:27" s="76" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="69">
+      <c r="J13" s="100" t="s">
+        <v>108</v>
+      </c>
+      <c r="M13" s="51"/>
+      <c r="N13" s="51"/>
+      <c r="O13" s="51"/>
+      <c r="P13" s="51"/>
+      <c r="Q13" s="51"/>
+      <c r="R13" s="51"/>
+      <c r="S13" s="51"/>
+      <c r="T13" s="51"/>
+      <c r="U13" s="51"/>
+      <c r="V13" s="51"/>
+      <c r="W13" s="51"/>
+      <c r="X13" s="51"/>
+      <c r="Y13" s="51"/>
+      <c r="Z13" s="51"/>
+      <c r="AA13" s="51"/>
+    </row>
+    <row r="14" spans="1:27" s="50" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A14" s="44">
         <v>10</v>
       </c>
-      <c r="B14" s="78" t="s">
+      <c r="B14" s="52" t="s">
         <v>93</v>
       </c>
-      <c r="C14" s="71" t="s">
+      <c r="C14" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="D14" s="86" t="s">
+      <c r="D14" s="57" t="s">
         <v>100</v>
       </c>
-      <c r="E14" s="87">
+      <c r="E14" s="58">
         <v>45017</v>
       </c>
-      <c r="F14" s="87">
+      <c r="F14" s="58">
         <v>45290</v>
       </c>
-      <c r="G14" s="71" t="s">
+      <c r="G14" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="H14" s="73" t="s">
+      <c r="H14" s="48" t="s">
         <v>103</v>
       </c>
-      <c r="I14" s="74">
+      <c r="I14" s="49">
         <v>79.900000000000006</v>
       </c>
-      <c r="J14" s="75"/>
-      <c r="M14" s="77"/>
-      <c r="N14" s="77"/>
-      <c r="O14" s="77"/>
-      <c r="P14" s="77"/>
-      <c r="Q14" s="77"/>
-      <c r="R14" s="77"/>
-      <c r="S14" s="77"/>
-      <c r="T14" s="77"/>
-      <c r="U14" s="77"/>
-      <c r="V14" s="77"/>
-      <c r="W14" s="77"/>
-      <c r="X14" s="77"/>
-      <c r="Y14" s="77"/>
-      <c r="Z14" s="77"/>
-      <c r="AA14" s="77"/>
-    </row>
-    <row r="15" spans="1:27" s="76" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="69">
+      <c r="J14" s="99" t="s">
+        <v>107</v>
+      </c>
+      <c r="M14" s="51"/>
+      <c r="N14" s="51"/>
+      <c r="O14" s="51"/>
+      <c r="P14" s="51"/>
+      <c r="Q14" s="51"/>
+      <c r="R14" s="51"/>
+      <c r="S14" s="51"/>
+      <c r="T14" s="51"/>
+      <c r="U14" s="51"/>
+      <c r="V14" s="51"/>
+      <c r="W14" s="51"/>
+      <c r="X14" s="51"/>
+      <c r="Y14" s="51"/>
+      <c r="Z14" s="51"/>
+      <c r="AA14" s="51"/>
+    </row>
+    <row r="15" spans="1:27" s="50" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="44">
         <v>11</v>
       </c>
-      <c r="B15" s="70" t="s">
+      <c r="B15" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="C15" s="71" t="s">
+      <c r="C15" s="46" t="s">
         <v>99</v>
       </c>
-      <c r="D15" s="86" t="s">
+      <c r="D15" s="57" t="s">
         <v>100</v>
       </c>
-      <c r="E15" s="87">
+      <c r="E15" s="58">
         <v>46419</v>
       </c>
-      <c r="F15" s="87">
+      <c r="F15" s="58">
         <v>46784</v>
       </c>
-      <c r="G15" s="71" t="s">
+      <c r="G15" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="H15" s="73" t="s">
+      <c r="H15" s="48" t="s">
         <v>104</v>
       </c>
-      <c r="I15" s="74">
+      <c r="I15" s="49">
         <v>0</v>
       </c>
-      <c r="J15" s="77"/>
-      <c r="M15" s="77"/>
-      <c r="N15" s="77"/>
-      <c r="O15" s="77"/>
-      <c r="P15" s="77"/>
-      <c r="Q15" s="77"/>
-      <c r="R15" s="77"/>
-      <c r="S15" s="77"/>
-      <c r="T15" s="77"/>
-      <c r="U15" s="77"/>
-      <c r="V15" s="77"/>
-      <c r="W15" s="77"/>
-      <c r="X15" s="77"/>
-      <c r="Y15" s="77"/>
-      <c r="Z15" s="77"/>
-      <c r="AA15" s="77"/>
-    </row>
-    <row r="16" spans="1:27" s="76" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="69"/>
-      <c r="B16" s="79"/>
-      <c r="C16" s="80"/>
-      <c r="D16" s="80"/>
-      <c r="E16" s="81"/>
-      <c r="F16" s="81"/>
-      <c r="G16" s="80"/>
-      <c r="H16" s="82"/>
-      <c r="I16" s="88"/>
-      <c r="J16" s="77"/>
-      <c r="M16" s="77"/>
-      <c r="N16" s="77"/>
-      <c r="O16" s="77"/>
-      <c r="P16" s="77"/>
-      <c r="Q16" s="77"/>
-      <c r="R16" s="77"/>
-      <c r="S16" s="77"/>
-      <c r="T16" s="77"/>
-      <c r="U16" s="77"/>
-      <c r="V16" s="77"/>
-      <c r="W16" s="77"/>
-      <c r="X16" s="77"/>
-      <c r="Y16" s="77"/>
-      <c r="Z16" s="77"/>
-      <c r="AA16" s="77"/>
-    </row>
-    <row r="17" spans="1:27" s="76" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="83"/>
-      <c r="B17" s="84"/>
-      <c r="C17" s="84"/>
-      <c r="D17" s="84"/>
-      <c r="E17" s="84"/>
-      <c r="F17" s="84"/>
-      <c r="G17" s="84"/>
-      <c r="H17" s="84"/>
-      <c r="I17" s="85"/>
-      <c r="J17" s="77"/>
-      <c r="L17" s="77"/>
-      <c r="M17" s="77"/>
-      <c r="N17" s="77"/>
-      <c r="O17" s="77"/>
-      <c r="P17" s="77"/>
-      <c r="Q17" s="77"/>
-      <c r="R17" s="77"/>
-      <c r="S17" s="77"/>
-      <c r="T17" s="77"/>
-      <c r="U17" s="77"/>
-      <c r="V17" s="77"/>
-      <c r="W17" s="77"/>
-      <c r="X17" s="77"/>
-      <c r="Y17" s="77"/>
-      <c r="Z17" s="77"/>
-      <c r="AA17" s="77"/>
-    </row>
-    <row r="18" spans="1:27" s="92" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="90"/>
-      <c r="B18" s="90"/>
-      <c r="C18" s="90"/>
-      <c r="D18" s="90"/>
-      <c r="E18" s="90"/>
-      <c r="F18" s="90"/>
-      <c r="G18" s="90"/>
-      <c r="H18" s="90"/>
-      <c r="I18" s="90"/>
-      <c r="J18" s="91"/>
-      <c r="L18" s="91"/>
-      <c r="M18" s="91"/>
-      <c r="N18" s="91"/>
-      <c r="O18" s="91"/>
-      <c r="P18" s="91"/>
-      <c r="Q18" s="91"/>
-      <c r="R18" s="91"/>
-      <c r="S18" s="91"/>
-      <c r="T18" s="91"/>
-      <c r="U18" s="91"/>
-      <c r="V18" s="91"/>
-      <c r="W18" s="91"/>
-      <c r="X18" s="91"/>
-      <c r="Y18" s="91"/>
-      <c r="Z18" s="91"/>
-      <c r="AA18" s="91"/>
-    </row>
-    <row r="19" spans="1:27" s="92" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="93" t="s">
+      <c r="J15" s="44"/>
+      <c r="M15" s="51"/>
+      <c r="N15" s="51"/>
+      <c r="O15" s="51"/>
+      <c r="P15" s="51"/>
+      <c r="Q15" s="51"/>
+      <c r="R15" s="51"/>
+      <c r="S15" s="51"/>
+      <c r="T15" s="51"/>
+      <c r="U15" s="51"/>
+      <c r="V15" s="51"/>
+      <c r="W15" s="51"/>
+      <c r="X15" s="51"/>
+      <c r="Y15" s="51"/>
+      <c r="Z15" s="51"/>
+      <c r="AA15" s="51"/>
+    </row>
+    <row r="16" spans="1:27" s="50" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A16" s="44"/>
+      <c r="B16" s="53"/>
+      <c r="C16" s="54"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="55"/>
+      <c r="F16" s="55"/>
+      <c r="G16" s="54"/>
+      <c r="H16" s="56"/>
+      <c r="I16" s="59"/>
+      <c r="J16" s="98"/>
+      <c r="M16" s="51"/>
+      <c r="N16" s="51"/>
+      <c r="O16" s="51"/>
+      <c r="P16" s="51"/>
+      <c r="Q16" s="51"/>
+      <c r="R16" s="51"/>
+      <c r="S16" s="51"/>
+      <c r="T16" s="51"/>
+      <c r="U16" s="51"/>
+      <c r="V16" s="51"/>
+      <c r="W16" s="51"/>
+      <c r="X16" s="51"/>
+      <c r="Y16" s="51"/>
+      <c r="Z16" s="51"/>
+      <c r="AA16" s="51"/>
+    </row>
+    <row r="17" spans="1:27" s="50" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A17" s="96"/>
+      <c r="B17" s="97"/>
+      <c r="C17" s="97"/>
+      <c r="D17" s="97"/>
+      <c r="E17" s="97"/>
+      <c r="F17" s="97"/>
+      <c r="G17" s="97"/>
+      <c r="H17" s="97"/>
+      <c r="I17" s="97"/>
+      <c r="J17" s="97"/>
+      <c r="K17" s="60"/>
+      <c r="L17" s="51"/>
+      <c r="M17" s="51"/>
+      <c r="N17" s="51"/>
+      <c r="O17" s="51"/>
+      <c r="P17" s="51"/>
+      <c r="Q17" s="51"/>
+      <c r="R17" s="51"/>
+      <c r="S17" s="51"/>
+      <c r="T17" s="51"/>
+      <c r="U17" s="51"/>
+      <c r="V17" s="51"/>
+      <c r="W17" s="51"/>
+      <c r="X17" s="51"/>
+      <c r="Y17" s="51"/>
+      <c r="Z17" s="51"/>
+      <c r="AA17" s="51"/>
+    </row>
+    <row r="18" spans="1:27" s="50" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="61"/>
+      <c r="B18" s="61"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="61"/>
+      <c r="E18" s="61"/>
+      <c r="F18" s="61"/>
+      <c r="G18" s="61"/>
+      <c r="H18" s="61"/>
+      <c r="I18" s="61"/>
+      <c r="J18" s="51"/>
+      <c r="L18" s="51"/>
+      <c r="M18" s="51"/>
+      <c r="N18" s="51"/>
+      <c r="O18" s="51"/>
+      <c r="P18" s="51"/>
+      <c r="Q18" s="51"/>
+      <c r="R18" s="51"/>
+      <c r="S18" s="51"/>
+      <c r="T18" s="51"/>
+      <c r="U18" s="51"/>
+      <c r="V18" s="51"/>
+      <c r="W18" s="51"/>
+      <c r="X18" s="51"/>
+      <c r="Y18" s="51"/>
+      <c r="Z18" s="51"/>
+      <c r="AA18" s="51"/>
+    </row>
+    <row r="19" spans="1:27" s="50" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="77" t="s">
         <v>106</v>
       </c>
-      <c r="B19" s="95" t="s">
+      <c r="B19" s="71" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="51" t="s">
+      <c r="C19" s="79" t="s">
         <v>46</v>
       </c>
-      <c r="D19" s="51"/>
-      <c r="E19" s="90"/>
-      <c r="F19" s="90"/>
-      <c r="G19" s="90"/>
-      <c r="H19" s="90"/>
-      <c r="I19" s="90"/>
-      <c r="J19" s="91"/>
-      <c r="L19" s="91"/>
-      <c r="M19" s="91"/>
-      <c r="N19" s="91"/>
-      <c r="O19" s="91"/>
-      <c r="P19" s="91"/>
-      <c r="Q19" s="91"/>
-      <c r="R19" s="91"/>
-      <c r="S19" s="91"/>
-      <c r="T19" s="91"/>
-      <c r="U19" s="91"/>
-      <c r="V19" s="91"/>
-      <c r="W19" s="91"/>
-      <c r="X19" s="91"/>
-      <c r="Y19" s="91"/>
-      <c r="Z19" s="91"/>
-      <c r="AA19" s="91"/>
-    </row>
-    <row r="20" spans="1:27" s="92" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="94"/>
-      <c r="B20" s="96"/>
+      <c r="D19" s="79"/>
+      <c r="E19" s="61"/>
+      <c r="F19" s="61"/>
+      <c r="G19" s="61"/>
+      <c r="H19" s="61"/>
+      <c r="I19" s="61"/>
+      <c r="J19" s="51"/>
+      <c r="L19" s="51"/>
+      <c r="M19" s="51"/>
+      <c r="N19" s="51"/>
+      <c r="O19" s="51"/>
+      <c r="P19" s="51"/>
+      <c r="Q19" s="51"/>
+      <c r="R19" s="51"/>
+      <c r="S19" s="51"/>
+      <c r="T19" s="51"/>
+      <c r="U19" s="51"/>
+      <c r="V19" s="51"/>
+      <c r="W19" s="51"/>
+      <c r="X19" s="51"/>
+      <c r="Y19" s="51"/>
+      <c r="Z19" s="51"/>
+      <c r="AA19" s="51"/>
+    </row>
+    <row r="20" spans="1:27" s="50" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="78"/>
+      <c r="B20" s="72"/>
       <c r="C20" s="22" t="s">
         <v>49</v>
       </c>
       <c r="D20" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="E20" s="97"/>
-      <c r="F20" s="90"/>
-      <c r="G20" s="90"/>
-      <c r="H20" s="90"/>
-      <c r="I20" s="90"/>
-      <c r="J20" s="91"/>
-      <c r="L20" s="91"/>
-      <c r="M20" s="91"/>
-      <c r="N20" s="91"/>
-      <c r="O20" s="91"/>
-      <c r="P20" s="91"/>
-      <c r="Q20" s="91"/>
-      <c r="R20" s="91"/>
-      <c r="S20" s="91"/>
-      <c r="T20" s="91"/>
-      <c r="U20" s="91"/>
-      <c r="V20" s="91"/>
-      <c r="W20" s="91"/>
-      <c r="X20" s="91"/>
-      <c r="Y20" s="91"/>
-      <c r="Z20" s="91"/>
-      <c r="AA20" s="91"/>
-    </row>
-    <row r="21" spans="1:27" s="92" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="69">
+      <c r="E20" s="62"/>
+      <c r="F20" s="61"/>
+      <c r="G20" s="61"/>
+      <c r="H20" s="61"/>
+      <c r="I20" s="61"/>
+      <c r="J20" s="51"/>
+      <c r="L20" s="51"/>
+      <c r="M20" s="51"/>
+      <c r="N20" s="51"/>
+      <c r="O20" s="51"/>
+      <c r="P20" s="51"/>
+      <c r="Q20" s="51"/>
+      <c r="R20" s="51"/>
+      <c r="S20" s="51"/>
+      <c r="T20" s="51"/>
+      <c r="U20" s="51"/>
+      <c r="V20" s="51"/>
+      <c r="W20" s="51"/>
+      <c r="X20" s="51"/>
+      <c r="Y20" s="51"/>
+      <c r="Z20" s="51"/>
+      <c r="AA20" s="51"/>
+    </row>
+    <row r="21" spans="1:27" s="50" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="44">
         <v>1</v>
       </c>
-      <c r="B21" s="70" t="s">
+      <c r="B21" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="C21" s="72">
+      <c r="C21" s="47">
         <v>45017</v>
       </c>
-      <c r="D21" s="72">
+      <c r="D21" s="47">
         <v>46148</v>
       </c>
-      <c r="E21" s="97"/>
-      <c r="F21" s="90"/>
-      <c r="G21" s="90"/>
-      <c r="H21" s="90"/>
-      <c r="I21" s="90"/>
-      <c r="J21" s="91"/>
-      <c r="L21" s="91"/>
-      <c r="M21" s="91"/>
-      <c r="N21" s="91"/>
-      <c r="O21" s="91"/>
-      <c r="P21" s="91"/>
-      <c r="Q21" s="91"/>
-      <c r="R21" s="91"/>
-      <c r="S21" s="91"/>
-      <c r="T21" s="91"/>
-      <c r="U21" s="91"/>
-      <c r="V21" s="91"/>
-      <c r="W21" s="91"/>
-      <c r="X21" s="91"/>
-      <c r="Y21" s="91"/>
-      <c r="Z21" s="91"/>
-      <c r="AA21" s="91"/>
-    </row>
-    <row r="22" spans="1:27" s="92" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="69">
+      <c r="E21" s="62"/>
+      <c r="F21" s="61"/>
+      <c r="G21" s="61"/>
+      <c r="H21" s="61"/>
+      <c r="I21" s="61"/>
+      <c r="J21" s="51"/>
+      <c r="L21" s="51"/>
+      <c r="M21" s="51"/>
+      <c r="N21" s="51"/>
+      <c r="O21" s="51"/>
+      <c r="P21" s="51"/>
+      <c r="Q21" s="51"/>
+      <c r="R21" s="51"/>
+      <c r="S21" s="51"/>
+      <c r="T21" s="51"/>
+      <c r="U21" s="51"/>
+      <c r="V21" s="51"/>
+      <c r="W21" s="51"/>
+      <c r="X21" s="51"/>
+      <c r="Y21" s="51"/>
+      <c r="Z21" s="51"/>
+      <c r="AA21" s="51"/>
+    </row>
+    <row r="22" spans="1:27" s="50" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A22" s="44">
         <v>2</v>
       </c>
-      <c r="B22" s="70" t="s">
+      <c r="B22" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="C22" s="72">
+      <c r="C22" s="47">
         <v>46419</v>
       </c>
-      <c r="D22" s="72">
+      <c r="D22" s="47">
         <v>46784</v>
       </c>
-      <c r="E22" s="90"/>
-      <c r="F22" s="90"/>
-      <c r="G22" s="90"/>
-      <c r="H22" s="90"/>
-      <c r="I22" s="90"/>
-      <c r="J22" s="91"/>
-      <c r="L22" s="91"/>
-      <c r="M22" s="91"/>
-      <c r="N22" s="91"/>
-      <c r="O22" s="91"/>
-      <c r="P22" s="91"/>
-      <c r="Q22" s="91"/>
-      <c r="R22" s="91"/>
-      <c r="S22" s="91"/>
-      <c r="T22" s="91"/>
-      <c r="U22" s="91"/>
-      <c r="V22" s="91"/>
-      <c r="W22" s="91"/>
-      <c r="X22" s="91"/>
-      <c r="Y22" s="91"/>
-      <c r="Z22" s="91"/>
-      <c r="AA22" s="91"/>
-    </row>
-    <row r="23" spans="1:27" s="92" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="90"/>
-      <c r="B23" s="90"/>
-      <c r="C23" s="90"/>
-      <c r="D23" s="90"/>
-      <c r="E23" s="90"/>
-      <c r="F23" s="90"/>
-      <c r="G23" s="90"/>
-      <c r="H23" s="90"/>
-      <c r="I23" s="90"/>
-      <c r="J23" s="91"/>
-      <c r="L23" s="91"/>
-      <c r="M23" s="91"/>
-      <c r="N23" s="91"/>
-      <c r="O23" s="91"/>
-      <c r="P23" s="91"/>
-      <c r="Q23" s="91"/>
-      <c r="R23" s="91"/>
-      <c r="S23" s="91"/>
-      <c r="T23" s="91"/>
-      <c r="U23" s="91"/>
-      <c r="V23" s="91"/>
-      <c r="W23" s="91"/>
-      <c r="X23" s="91"/>
-      <c r="Y23" s="91"/>
-      <c r="Z23" s="91"/>
-      <c r="AA23" s="91"/>
+      <c r="E22" s="61"/>
+      <c r="F22" s="61"/>
+      <c r="G22" s="61"/>
+      <c r="H22" s="61"/>
+      <c r="I22" s="61"/>
+      <c r="J22" s="51"/>
+      <c r="L22" s="51"/>
+      <c r="M22" s="51"/>
+      <c r="N22" s="51"/>
+      <c r="O22" s="51"/>
+      <c r="P22" s="51"/>
+      <c r="Q22" s="51"/>
+      <c r="R22" s="51"/>
+      <c r="S22" s="51"/>
+      <c r="T22" s="51"/>
+      <c r="U22" s="51"/>
+      <c r="V22" s="51"/>
+      <c r="W22" s="51"/>
+      <c r="X22" s="51"/>
+      <c r="Y22" s="51"/>
+      <c r="Z22" s="51"/>
+      <c r="AA22" s="51"/>
+    </row>
+    <row r="23" spans="1:27" s="50" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A23" s="61"/>
+      <c r="B23" s="61"/>
+      <c r="C23" s="61"/>
+      <c r="D23" s="61"/>
+      <c r="E23" s="61"/>
+      <c r="F23" s="61"/>
+      <c r="G23" s="61"/>
+      <c r="H23" s="61"/>
+      <c r="I23" s="61"/>
+      <c r="J23" s="51"/>
+      <c r="L23" s="51"/>
+      <c r="M23" s="51"/>
+      <c r="N23" s="51"/>
+      <c r="O23" s="51"/>
+      <c r="P23" s="51"/>
+      <c r="Q23" s="51"/>
+      <c r="R23" s="51"/>
+      <c r="S23" s="51"/>
+      <c r="T23" s="51"/>
+      <c r="U23" s="51"/>
+      <c r="V23" s="51"/>
+      <c r="W23" s="51"/>
+      <c r="X23" s="51"/>
+      <c r="Y23" s="51"/>
+      <c r="Z23" s="51"/>
+      <c r="AA23" s="51"/>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" s="39" t="s">
@@ -4210,16 +4258,16 @@
       <c r="A25" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="57" t="s">
+      <c r="B25" s="76" t="s">
         <v>70</v>
       </c>
-      <c r="C25" s="57"/>
-      <c r="D25" s="57"/>
-      <c r="E25" s="57"/>
-      <c r="F25" s="57"/>
-      <c r="G25" s="57"/>
-      <c r="H25" s="57"/>
-      <c r="I25" s="57"/>
+      <c r="C25" s="76"/>
+      <c r="D25" s="76"/>
+      <c r="E25" s="76"/>
+      <c r="F25" s="76"/>
+      <c r="G25" s="76"/>
+      <c r="H25" s="76"/>
+      <c r="I25" s="76"/>
       <c r="J25" s="16"/>
       <c r="K25" s="16"/>
       <c r="L25" s="16"/>
@@ -4243,16 +4291,16 @@
       <c r="A26" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="B26" s="57" t="s">
+      <c r="B26" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="C26" s="57"/>
-      <c r="D26" s="57"/>
-      <c r="E26" s="57"/>
-      <c r="F26" s="57"/>
-      <c r="G26" s="57"/>
-      <c r="H26" s="57"/>
-      <c r="I26" s="57"/>
+      <c r="C26" s="76"/>
+      <c r="D26" s="76"/>
+      <c r="E26" s="76"/>
+      <c r="F26" s="76"/>
+      <c r="G26" s="76"/>
+      <c r="H26" s="76"/>
+      <c r="I26" s="76"/>
       <c r="J26" s="16"/>
       <c r="K26" s="16"/>
       <c r="L26" s="16"/>
@@ -4276,16 +4324,16 @@
       <c r="A27" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="B27" s="57" t="s">
+      <c r="B27" s="76" t="s">
         <v>69</v>
       </c>
-      <c r="C27" s="57"/>
-      <c r="D27" s="57"/>
-      <c r="E27" s="57"/>
-      <c r="F27" s="57"/>
-      <c r="G27" s="57"/>
-      <c r="H27" s="57"/>
-      <c r="I27" s="57"/>
+      <c r="C27" s="76"/>
+      <c r="D27" s="76"/>
+      <c r="E27" s="76"/>
+      <c r="F27" s="76"/>
+      <c r="G27" s="76"/>
+      <c r="H27" s="76"/>
+      <c r="I27" s="76"/>
       <c r="J27" s="16"/>
       <c r="K27" s="16"/>
       <c r="L27" s="16"/>
@@ -4309,16 +4357,16 @@
       <c r="A28" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="57" t="s">
+      <c r="B28" s="76" t="s">
         <v>72</v>
       </c>
-      <c r="C28" s="57"/>
-      <c r="D28" s="57"/>
-      <c r="E28" s="57"/>
-      <c r="F28" s="57"/>
-      <c r="G28" s="57"/>
-      <c r="H28" s="57"/>
-      <c r="I28" s="57"/>
+      <c r="C28" s="76"/>
+      <c r="D28" s="76"/>
+      <c r="E28" s="76"/>
+      <c r="F28" s="76"/>
+      <c r="G28" s="76"/>
+      <c r="H28" s="76"/>
+      <c r="I28" s="76"/>
       <c r="J28" s="16"/>
       <c r="K28" s="16"/>
       <c r="L28" s="16"/>
@@ -4342,16 +4390,16 @@
       <c r="A29" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="B29" s="57" t="s">
+      <c r="B29" s="76" t="s">
         <v>71</v>
       </c>
-      <c r="C29" s="57"/>
-      <c r="D29" s="57"/>
-      <c r="E29" s="57"/>
-      <c r="F29" s="57"/>
-      <c r="G29" s="57"/>
-      <c r="H29" s="57"/>
-      <c r="I29" s="57"/>
+      <c r="C29" s="76"/>
+      <c r="D29" s="76"/>
+      <c r="E29" s="76"/>
+      <c r="F29" s="76"/>
+      <c r="G29" s="76"/>
+      <c r="H29" s="76"/>
+      <c r="I29" s="76"/>
       <c r="J29" s="16"/>
       <c r="K29" s="16"/>
       <c r="L29" s="16"/>
@@ -4375,16 +4423,16 @@
       <c r="A30" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="57" t="s">
+      <c r="B30" s="76" t="s">
         <v>73</v>
       </c>
-      <c r="C30" s="57"/>
-      <c r="D30" s="57"/>
-      <c r="E30" s="57"/>
-      <c r="F30" s="57"/>
-      <c r="G30" s="57"/>
-      <c r="H30" s="57"/>
-      <c r="I30" s="57"/>
+      <c r="C30" s="76"/>
+      <c r="D30" s="76"/>
+      <c r="E30" s="76"/>
+      <c r="F30" s="76"/>
+      <c r="G30" s="76"/>
+      <c r="H30" s="76"/>
+      <c r="I30" s="76"/>
       <c r="J30" s="16"/>
       <c r="K30" s="16"/>
       <c r="L30" s="16"/>
@@ -4408,16 +4456,16 @@
       <c r="A31" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="B31" s="57" t="s">
+      <c r="B31" s="76" t="s">
         <v>74</v>
       </c>
-      <c r="C31" s="57"/>
-      <c r="D31" s="57"/>
-      <c r="E31" s="57"/>
-      <c r="F31" s="57"/>
-      <c r="G31" s="57"/>
-      <c r="H31" s="57"/>
-      <c r="I31" s="57"/>
+      <c r="C31" s="76"/>
+      <c r="D31" s="76"/>
+      <c r="E31" s="76"/>
+      <c r="F31" s="76"/>
+      <c r="G31" s="76"/>
+      <c r="H31" s="76"/>
+      <c r="I31" s="76"/>
       <c r="J31" s="16"/>
       <c r="K31" s="16"/>
       <c r="L31" s="16"/>
@@ -4499,14 +4547,14 @@
     </row>
     <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34" s="41"/>
-      <c r="B34" s="58"/>
-      <c r="C34" s="59"/>
-      <c r="D34" s="59"/>
-      <c r="E34" s="59"/>
-      <c r="F34" s="59"/>
-      <c r="G34" s="59"/>
-      <c r="H34" s="59"/>
-      <c r="I34" s="60"/>
+      <c r="B34" s="80"/>
+      <c r="C34" s="81"/>
+      <c r="D34" s="81"/>
+      <c r="E34" s="81"/>
+      <c r="F34" s="81"/>
+      <c r="G34" s="81"/>
+      <c r="H34" s="81"/>
+      <c r="I34" s="82"/>
       <c r="J34" s="16"/>
       <c r="K34" s="16"/>
       <c r="L34" s="16"/>
@@ -4527,29 +4575,29 @@
       <c r="AA34" s="16"/>
     </row>
     <row r="35" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A35" s="61" t="s">
+      <c r="A35" s="83" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="63" t="s">
+      <c r="B35" s="85" t="s">
         <v>43</v>
       </c>
-      <c r="C35" s="63" t="s">
+      <c r="C35" s="85" t="s">
         <v>44</v>
       </c>
-      <c r="D35" s="63" t="s">
+      <c r="D35" s="85" t="s">
         <v>45</v>
       </c>
-      <c r="E35" s="65" t="s">
+      <c r="E35" s="87" t="s">
         <v>46</v>
       </c>
-      <c r="F35" s="66"/>
-      <c r="G35" s="63" t="s">
+      <c r="F35" s="88"/>
+      <c r="G35" s="85" t="s">
         <v>67</v>
       </c>
-      <c r="H35" s="63" t="s">
+      <c r="H35" s="85" t="s">
         <v>47</v>
       </c>
-      <c r="I35" s="67" t="s">
+      <c r="I35" s="89" t="s">
         <v>48</v>
       </c>
       <c r="J35" s="16"/>
@@ -4572,19 +4620,19 @@
       <c r="AA35" s="16"/>
     </row>
     <row r="36" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A36" s="62"/>
-      <c r="B36" s="64"/>
-      <c r="C36" s="64"/>
-      <c r="D36" s="64"/>
+      <c r="A36" s="84"/>
+      <c r="B36" s="86"/>
+      <c r="C36" s="86"/>
+      <c r="D36" s="86"/>
       <c r="E36" s="23" t="s">
         <v>49</v>
       </c>
       <c r="F36" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="G36" s="64"/>
-      <c r="H36" s="64"/>
-      <c r="I36" s="68"/>
+      <c r="G36" s="86"/>
+      <c r="H36" s="86"/>
+      <c r="I36" s="90"/>
       <c r="J36" s="16"/>
       <c r="K36" s="16"/>
       <c r="L36" s="16"/>
@@ -4652,15 +4700,15 @@
       <c r="AA37" s="16"/>
     </row>
     <row r="38" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A38" s="53"/>
-      <c r="B38" s="54"/>
-      <c r="C38" s="54"/>
-      <c r="D38" s="54"/>
-      <c r="E38" s="54"/>
-      <c r="F38" s="54"/>
-      <c r="G38" s="54"/>
-      <c r="H38" s="54"/>
-      <c r="I38" s="55"/>
+      <c r="A38" s="73"/>
+      <c r="B38" s="74"/>
+      <c r="C38" s="74"/>
+      <c r="D38" s="74"/>
+      <c r="E38" s="74"/>
+      <c r="F38" s="74"/>
+      <c r="G38" s="74"/>
+      <c r="H38" s="74"/>
+      <c r="I38" s="75"/>
       <c r="J38" s="16"/>
       <c r="K38" s="16"/>
       <c r="L38" s="16"/>
@@ -4741,16 +4789,16 @@
       <c r="AA40" s="16"/>
     </row>
     <row r="41" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A41" s="57" t="s">
+      <c r="A41" s="76" t="s">
         <v>77</v>
       </c>
-      <c r="B41" s="57"/>
-      <c r="C41" s="57"/>
-      <c r="D41" s="57"/>
-      <c r="E41" s="57"/>
-      <c r="F41" s="57"/>
-      <c r="G41" s="57"/>
-      <c r="H41" s="57"/>
+      <c r="B41" s="76"/>
+      <c r="C41" s="76"/>
+      <c r="D41" s="76"/>
+      <c r="E41" s="76"/>
+      <c r="F41" s="76"/>
+      <c r="G41" s="76"/>
+      <c r="H41" s="76"/>
       <c r="I41" s="16"/>
       <c r="J41" s="16"/>
       <c r="K41" s="16"/>
@@ -4772,16 +4820,16 @@
       <c r="AA41" s="16"/>
     </row>
     <row r="42" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A42" s="57" t="s">
+      <c r="A42" s="76" t="s">
         <v>76</v>
       </c>
-      <c r="B42" s="57"/>
-      <c r="C42" s="57"/>
-      <c r="D42" s="57"/>
-      <c r="E42" s="57"/>
-      <c r="F42" s="57"/>
-      <c r="G42" s="57"/>
-      <c r="H42" s="57"/>
+      <c r="B42" s="76"/>
+      <c r="C42" s="76"/>
+      <c r="D42" s="76"/>
+      <c r="E42" s="76"/>
+      <c r="F42" s="76"/>
+      <c r="G42" s="76"/>
+      <c r="H42" s="76"/>
       <c r="I42" s="16"/>
       <c r="J42" s="16"/>
       <c r="K42" s="16"/>
@@ -4803,16 +4851,16 @@
       <c r="AA42" s="16"/>
     </row>
     <row r="43" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A43" s="57" t="s">
+      <c r="A43" s="76" t="s">
         <v>105</v>
       </c>
-      <c r="B43" s="57"/>
-      <c r="C43" s="57"/>
-      <c r="D43" s="57"/>
-      <c r="E43" s="57"/>
-      <c r="F43" s="57"/>
-      <c r="G43" s="57"/>
-      <c r="H43" s="57"/>
+      <c r="B43" s="76"/>
+      <c r="C43" s="76"/>
+      <c r="D43" s="76"/>
+      <c r="E43" s="76"/>
+      <c r="F43" s="76"/>
+      <c r="G43" s="76"/>
+      <c r="H43" s="76"/>
       <c r="I43" s="16"/>
       <c r="J43" s="16"/>
       <c r="K43" s="16"/>
@@ -4834,16 +4882,16 @@
       <c r="AA43" s="16"/>
     </row>
     <row r="44" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A44" s="57" t="s">
+      <c r="A44" s="76" t="s">
         <v>75</v>
       </c>
-      <c r="B44" s="57"/>
-      <c r="C44" s="57"/>
-      <c r="D44" s="57"/>
-      <c r="E44" s="57"/>
-      <c r="F44" s="57"/>
-      <c r="G44" s="57"/>
-      <c r="H44" s="57"/>
+      <c r="B44" s="76"/>
+      <c r="C44" s="76"/>
+      <c r="D44" s="76"/>
+      <c r="E44" s="76"/>
+      <c r="F44" s="76"/>
+      <c r="G44" s="76"/>
+      <c r="H44" s="76"/>
       <c r="I44" s="16"/>
       <c r="J44" s="16"/>
       <c r="K44" s="16"/>
@@ -32676,22 +32724,19 @@
       <c r="AA1003" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="35">
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="A17:I17"/>
-    <mergeCell ref="A38:I38"/>
-    <mergeCell ref="A41:H41"/>
-    <mergeCell ref="A42:H42"/>
-    <mergeCell ref="A43:H43"/>
-    <mergeCell ref="B30:I30"/>
-    <mergeCell ref="B31:I31"/>
-    <mergeCell ref="B25:I25"/>
-    <mergeCell ref="B26:I26"/>
-    <mergeCell ref="B27:I27"/>
-    <mergeCell ref="B28:I28"/>
-    <mergeCell ref="B29:I29"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="C19:D19"/>
+  <mergeCells count="36">
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A17:J17"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
     <mergeCell ref="A44:H44"/>
     <mergeCell ref="B34:I34"/>
     <mergeCell ref="A35:A36"/>
@@ -32702,16 +32747,20 @@
     <mergeCell ref="G35:G36"/>
     <mergeCell ref="H35:H36"/>
     <mergeCell ref="I35:I36"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="A43:H43"/>
+    <mergeCell ref="B30:I30"/>
+    <mergeCell ref="B31:I31"/>
+    <mergeCell ref="B25:I25"/>
+    <mergeCell ref="B26:I26"/>
+    <mergeCell ref="B27:I27"/>
+    <mergeCell ref="B28:I28"/>
+    <mergeCell ref="B29:I29"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="A38:I38"/>
+    <mergeCell ref="A41:H41"/>
+    <mergeCell ref="A42:H42"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="C19:D19"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>